<commit_message>
Finalized cases for MSI, MESI and MOSI
</commit_message>
<xml_diff>
--- a/protocol_testcase.xlsx
+++ b/protocol_testcase.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shahm\OneDrive\Documents\GitHub\cache-coherence-simulator\240b\cache-coherence-simulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gandhardeshpande/Desktop/CSE240B/Project/cache-coherence-simulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F43F5DD-0273-4DF2-B4EA-5D3C6B60FBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512FD6D0-15E7-A441-88C7-69F09E4FC4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{B53E9CC3-ECBE-4745-AC74-EE8F4F913379}"/>
+    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{B53E9CC3-ECBE-4745-AC74-EE8F4F913379}"/>
   </bookViews>
   <sheets>
-    <sheet name="MESI" sheetId="1" r:id="rId1"/>
-    <sheet name="MOSI" sheetId="2" r:id="rId2"/>
-    <sheet name="MOESI" sheetId="4" r:id="rId3"/>
-    <sheet name="Statistics" sheetId="5" r:id="rId4"/>
+    <sheet name="MSI" sheetId="6" r:id="rId1"/>
+    <sheet name="MESI" sheetId="1" r:id="rId2"/>
+    <sheet name="MOSI" sheetId="2" r:id="rId3"/>
+    <sheet name="MOESI" sheetId="4" r:id="rId4"/>
+    <sheet name="Statistics" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MESI!$A$1:$A$65</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MOESI!$A$1:$A$101</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MOSI!$A$1:$A$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MESI!$A$1:$A$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MOESI!$A$1:$A$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MOSI!$A$1:$A$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="46">
   <si>
     <t>Operation</t>
   </si>
@@ -154,6 +154,33 @@
   </si>
   <si>
     <t>POLLOTHERS</t>
+  </si>
+  <si>
+    <t>Validity</t>
+  </si>
+  <si>
+    <t>HIT/MISS</t>
+  </si>
+  <si>
+    <t>Private state</t>
+  </si>
+  <si>
+    <t>Sent state</t>
+  </si>
+  <si>
+    <t>Other state</t>
+  </si>
+  <si>
+    <t>Other state variation</t>
+  </si>
+  <si>
+    <t>Covered access</t>
+  </si>
+  <si>
+    <t>Covered Action</t>
+  </si>
+  <si>
+    <t>To check</t>
   </si>
 </sst>
 </file>
@@ -504,23 +531,823 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5E4DA1-78E6-844B-B642-01D16D60A9E0}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5424022-4FB1-44DF-AF4A-94A16CC54A36}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.59765625" customWidth="1"/>
-    <col min="7" max="7" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -555,7 +1382,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -572,7 +1399,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -589,7 +1416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -606,7 +1433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -623,7 +1450,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -649,7 +1476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -675,7 +1502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -692,7 +1519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -709,7 +1536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -735,7 +1562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -752,7 +1579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -769,7 +1596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -786,7 +1613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -812,7 +1639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -829,7 +1656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -846,7 +1673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -863,7 +1690,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -895,7 +1722,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -924,7 +1751,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -953,7 +1780,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -985,7 +1812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1002,7 +1829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1019,7 +1846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1036,7 +1863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1053,7 +1880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1070,7 +1897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1087,7 +1914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1104,7 +1931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1121,7 +1948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1138,7 +1965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1155,7 +1982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1172,7 +1999,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1189,7 +2016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -1206,7 +2033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1223,7 +2050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1240,7 +2067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1257,7 +2084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -1283,7 +2110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -1309,7 +2136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1326,7 +2153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1343,7 +2170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -1369,7 +2196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1386,7 +2213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -1403,7 +2230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -1420,7 +2247,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -1446,7 +2273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -1463,7 +2290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -1480,7 +2307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -1497,7 +2324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -1523,7 +2350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -1549,7 +2376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -1575,7 +2402,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -1601,7 +2428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -1618,7 +2445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -1635,7 +2462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -1652,7 +2479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -1669,7 +2496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -1686,7 +2513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -1703,7 +2530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -1720,7 +2547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -1737,7 +2564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -1754,7 +2581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -1771,7 +2598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -1788,7 +2615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -1811,17 +2638,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF618FD6-2D0C-41D0-9C29-911670B0073B}">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView topLeftCell="A25" zoomScale="159" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1856,7 +2683,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1873,7 +2700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1890,7 +2717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1907,7 +2734,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1924,7 +2751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1950,7 +2777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1976,7 +2803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2002,7 +2829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2019,7 +2846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2045,7 +2872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2071,7 +2898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2088,7 +2915,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2105,7 +2932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2131,7 +2958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2148,7 +2975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2165,7 +2992,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2182,7 +3009,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2208,7 +3035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2234,7 +3061,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2266,7 +3093,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -2298,7 +3125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2315,7 +3142,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -2332,7 +3159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -2349,7 +3176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2366,7 +3193,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2383,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2400,7 +3227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2417,7 +3244,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2434,7 +3261,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2451,7 +3278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2468,7 +3295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -2485,7 +3312,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2502,7 +3329,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2519,7 +3346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2536,7 +3363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2553,7 +3380,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2570,7 +3397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -2596,7 +3423,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -2622,7 +3449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -2648,9 +3475,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
         <v>13</v>
@@ -2673,8 +3500,11 @@
       <c r="H41" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="L41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -2700,7 +3530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -2726,7 +3556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -2743,7 +3573,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2760,7 +3590,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -2786,7 +3616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2803,7 +3633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -2820,7 +3650,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -2837,7 +3667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -2863,7 +3693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -2889,7 +3719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -2915,7 +3745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -2941,7 +3771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -2958,7 +3788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -2975,7 +3805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -2992,7 +3822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -3009,7 +3839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3026,7 +3856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3043,7 +3873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -3060,7 +3890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3077,7 +3907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3094,7 +3924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3111,7 +3941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -3128,7 +3958,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -3151,21 +3981,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79410132-39F9-44D5-8B09-6F0C28D6372B}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3200,7 +4029,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3217,7 +4046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3234,7 +4063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3251,7 +4080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3268,7 +4097,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3285,7 +4114,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -3311,7 +4140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -3337,7 +4166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3354,7 +4183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3380,7 +4209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3397,7 +4226,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3423,7 +4252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -3440,7 +4269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3457,7 +4286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3474,7 +4303,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3491,7 +4320,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3517,7 +4346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3543,7 +4372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -3560,7 +4389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -3577,7 +4406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -3594,7 +4423,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -3620,7 +4449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -3637,7 +4466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -3654,7 +4483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -3671,7 +4500,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -3688,7 +4517,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -3714,7 +4543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -3740,7 +4569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -3766,7 +4595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -3792,7 +4621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -3818,7 +4647,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -3835,7 +4664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -3852,7 +4681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -3869,7 +4698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -3886,7 +4715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -3903,7 +4732,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -3920,7 +4749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -3937,7 +4766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3954,7 +4783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -3971,7 +4800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3988,7 +4817,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -4005,7 +4834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -4022,7 +4851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -4039,7 +4868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -4056,7 +4885,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -4073,7 +4902,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -4090,7 +4919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -4107,7 +4936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -4124,7 +4953,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -4141,7 +4970,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -4158,7 +4987,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -4175,7 +5004,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -4192,7 +5021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -4209,7 +5038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -4226,7 +5055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -4243,7 +5072,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -4269,7 +5098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -4295,7 +5124,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -4312,7 +5141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -4338,7 +5167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -4355,7 +5184,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -4381,7 +5210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -4398,7 +5227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -4415,7 +5244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -4432,7 +5261,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -4449,7 +5278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -4475,7 +5304,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -4501,7 +5330,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -4518,7 +5347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -4535,7 +5364,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -4552,7 +5381,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -4578,7 +5407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -4595,7 +5424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4612,7 +5441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4629,7 +5458,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4646,7 +5475,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -4672,7 +5501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -4698,7 +5527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -4724,7 +5553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -4750,7 +5579,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>15</v>
       </c>
@@ -4776,7 +5605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4793,7 +5622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4810,7 +5639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4827,7 +5656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4844,7 +5673,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -4861,7 +5690,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4878,7 +5707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -4895,7 +5724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -4912,7 +5741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -4929,7 +5758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -4946,7 +5775,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -4963,7 +5792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -4980,7 +5809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>14</v>
       </c>
@@ -4997,7 +5826,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -5014,7 +5843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -5031,7 +5860,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -5048,7 +5877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -5065,7 +5894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -5082,7 +5911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -5099,7 +5928,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>14</v>
       </c>
@@ -5117,18 +5946,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A101" xr:uid="{79410132-39F9-44D5-8B09-6F0C28D6372B}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Y"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:A101" xr:uid="{79410132-39F9-44D5-8B09-6F0C28D6372B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF004507-2E17-4D0F-A673-D693F0BE6B39}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -5136,27 +5959,27 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>

</xml_diff>